<commit_message>
prepared for the strategy document
</commit_message>
<xml_diff>
--- a/Public_data/Exports_CDW_part1/actor_roles_summary.xlsx
+++ b/Public_data/Exports_CDW_part1/actor_roles_summary.xlsx
@@ -388,6 +388,9 @@
     <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker</t>
   </si>
   <si>
+    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker</t>
+  </si>
+  <si>
     <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker</t>
   </si>
   <si>
@@ -479,9 +482,6 @@
   </si>
   <si>
     <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker</t>
   </si>
   <si>
     <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Verwerker, Verwerker, Verwerker, Verwerker</t>
@@ -1341,7 +1341,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>35627</v>
+        <v>35646</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1349,7 +1349,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>3868</v>
+        <v>3874</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1357,7 +1357,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>985</v>
+        <v>987</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1365,7 +1365,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>458</v>
+        <v>460</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1381,7 +1381,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1477,7 +1477,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>3353</v>
+        <v>3476</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1485,7 +1485,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>4162</v>
+        <v>4144</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1493,7 +1493,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1509,7 +1509,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1517,7 +1517,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -1781,7 +1781,7 @@
         <v>56</v>
       </c>
       <c r="B57">
-        <v>847</v>
+        <v>884</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -1789,7 +1789,7 @@
         <v>57</v>
       </c>
       <c r="B58">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -1797,7 +1797,7 @@
         <v>58</v>
       </c>
       <c r="B59">
-        <v>1704</v>
+        <v>1693</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -1805,7 +1805,7 @@
         <v>59</v>
       </c>
       <c r="B60">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -1813,7 +1813,7 @@
         <v>60</v>
       </c>
       <c r="B61">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -1829,7 +1829,7 @@
         <v>62</v>
       </c>
       <c r="B63">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -1997,7 +1997,7 @@
         <v>83</v>
       </c>
       <c r="B84">
-        <v>322</v>
+        <v>340</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -2005,7 +2005,7 @@
         <v>84</v>
       </c>
       <c r="B85">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -2013,7 +2013,7 @@
         <v>85</v>
       </c>
       <c r="B86">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -2021,7 +2021,7 @@
         <v>86</v>
       </c>
       <c r="B87">
-        <v>1010</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -2029,7 +2029,7 @@
         <v>87</v>
       </c>
       <c r="B88">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -2045,7 +2045,7 @@
         <v>89</v>
       </c>
       <c r="B90">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -2253,7 +2253,7 @@
         <v>115</v>
       </c>
       <c r="B116">
-        <v>158</v>
+        <v>166</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -2269,7 +2269,7 @@
         <v>117</v>
       </c>
       <c r="B118">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -2277,7 +2277,7 @@
         <v>118</v>
       </c>
       <c r="B119">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -2285,7 +2285,7 @@
         <v>119</v>
       </c>
       <c r="B120">
-        <v>767</v>
+        <v>761</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -2293,7 +2293,7 @@
         <v>120</v>
       </c>
       <c r="B121">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -2301,7 +2301,7 @@
         <v>121</v>
       </c>
       <c r="B122">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -2349,7 +2349,7 @@
         <v>127</v>
       </c>
       <c r="B128">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -2357,7 +2357,7 @@
         <v>128</v>
       </c>
       <c r="B129">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -2413,7 +2413,7 @@
         <v>135</v>
       </c>
       <c r="B136">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -2421,7 +2421,7 @@
         <v>136</v>
       </c>
       <c r="B137">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -2429,7 +2429,7 @@
         <v>137</v>
       </c>
       <c r="B138">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -2437,7 +2437,7 @@
         <v>138</v>
       </c>
       <c r="B139">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -2445,7 +2445,7 @@
         <v>139</v>
       </c>
       <c r="B140">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -2477,7 +2477,7 @@
         <v>143</v>
       </c>
       <c r="B144">
-        <v>86</v>
+        <v>1</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -2485,7 +2485,7 @@
         <v>144</v>
       </c>
       <c r="B145">
-        <v>27</v>
+        <v>90</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -2493,7 +2493,7 @@
         <v>145</v>
       </c>
       <c r="B146">
-        <v>46</v>
+        <v>27</v>
       </c>
     </row>
     <row r="147" spans="1:2">
@@ -2501,7 +2501,7 @@
         <v>146</v>
       </c>
       <c r="B147">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="148" spans="1:2">
@@ -2509,7 +2509,7 @@
         <v>147</v>
       </c>
       <c r="B148">
-        <v>113</v>
+        <v>56</v>
       </c>
     </row>
     <row r="149" spans="1:2">
@@ -2517,7 +2517,7 @@
         <v>148</v>
       </c>
       <c r="B149">
-        <v>789</v>
+        <v>112</v>
       </c>
     </row>
     <row r="150" spans="1:2">
@@ -2525,7 +2525,7 @@
         <v>149</v>
       </c>
       <c r="B150">
-        <v>6</v>
+        <v>786</v>
       </c>
     </row>
     <row r="151" spans="1:2">
@@ -2533,7 +2533,7 @@
         <v>150</v>
       </c>
       <c r="B151">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="152" spans="1:2">
@@ -2685,7 +2685,7 @@
         <v>169</v>
       </c>
       <c r="B170">
-        <v>117</v>
+        <v>138</v>
       </c>
     </row>
     <row r="171" spans="1:2">
@@ -2701,7 +2701,7 @@
         <v>171</v>
       </c>
       <c r="B172">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="173" spans="1:2">
@@ -2733,7 +2733,7 @@
         <v>175</v>
       </c>
       <c r="B176">
-        <v>1831</v>
+        <v>1827</v>
       </c>
     </row>
     <row r="177" spans="1:2">

</xml_diff>